<commit_message>
- Change dB_MachAddChart to create the additional database entry to include the drive number in the entry - Added dB function to delete database item entry (have to do it via Excel functions rather than SQL). - Added dB function to delete an entire database - Modified dB_Query to automatically add the dB file extension (.xlsx) to the connection string rather than build it before every query, there's no point to that. - Capture database error message string and add it to the error message box when a database query fails - Add functionality to protect parameter chart part number entry when the delete and load buttons are not visible to prevent user entry - Changed the Machine Drive Name to a textbox from a combobox to just show the name rather than allow selection based on the name. - Simplified the machine selection change to update the chart info in a separate function. - Added functionality to overwrite an existing chart - Added functionality to delete and existing chart
</commit_message>
<xml_diff>
--- a/V1000_Drive_Programmer/data/M2100_CHARTS.XLSX
+++ b/V1000_Drive_Programmer/data/M2100_CHARTS.XLSX
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="23025" windowHeight="9870"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="22065" windowHeight="9870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>IDX</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>CHRT_DSC</t>
+  </si>
+  <si>
+    <t>64275_1</t>
   </si>
 </sst>
 </file>
@@ -348,14 +351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row spans="1:3" x14ac:dyDescent="0.2" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -366,11 +369,9 @@
         <v>2</v>
       </c>
     </row>
-    <row outlineLevel="0" r="2">
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>64275</t>
-        </is>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>